<commit_message>
changes to excel files of maps
</commit_message>
<xml_diff>
--- a/shinyapp/data/Sterling_Youth_Development 3.xlsx
+++ b/shinyapp/data/Sterling_Youth_Development 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78C83608-0B1F-D340-BEC4-86EC4F0A89BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A364F354-7501-EB44-8043-F0FE83B1D9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="124">
   <si>
-    <t>Longitude</t>
-  </si>
-  <si>
     <t>Costco</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>20908 Ashburn Road, Ashburn, VA 20147, United States of America</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
     <t>M-F: 10:00AM - 8:30PM</t>
   </si>
   <si>
@@ -231,9 +225,6 @@
     <t>M-F 7:00AM - 6:00PM</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Parks, Recreation and Community Services</t>
   </si>
   <si>
@@ -393,19 +384,28 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Hours</t>
+    <t>Name3</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>Website3</t>
+  </si>
+  <si>
+    <t>Latitude3</t>
+  </si>
+  <si>
+    <t>Longitude3</t>
+  </si>
+  <si>
+    <t>Description3</t>
+  </si>
+  <si>
+    <t>Hours3</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,25 +840,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
         <v>120</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>121</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
       </c>
       <c r="H1" t="s">
         <v>122</v>
@@ -869,16 +869,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -890,24 +890,24 @@
         <v>-77.555258699999996</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -919,24 +919,24 @@
         <v>-77.552453999999997</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -948,24 +948,24 @@
         <v>-77.555297999999993</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -977,24 +977,24 @@
         <v>-77.553653999999995</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1006,24 +1006,24 @@
         <v>-77.375861999999998</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1035,24 +1035,24 @@
         <v>-77.358749000000003</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1064,24 +1064,24 @@
         <v>-77.3927944</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1093,21 +1093,21 @@
         <v>-77.486816000000005</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1119,24 +1119,24 @@
         <v>-77.520797999999999</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1148,24 +1148,24 @@
         <v>-77.310794000000001</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1177,21 +1177,21 @@
         <v>-77.408413999999993</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1203,24 +1203,24 @@
         <v>-77.400994999999995</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1232,24 +1232,24 @@
         <v>-77.405699999999996</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1261,24 +1261,24 @@
         <v>-77.565443999999999</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -1290,24 +1290,24 @@
         <v>-77.346993999999995</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1319,24 +1319,24 @@
         <v>-77.406756999999999</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1348,24 +1348,24 @@
         <v>-77.499871799999994</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E19" s="2">
         <v>1</v>
@@ -1377,24 +1377,24 @@
         <v>-77.368133999999998</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -1406,24 +1406,24 @@
         <v>-77.149856999999997</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
@@ -1435,24 +1435,24 @@
         <v>-77.040006199999993</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -1464,24 +1464,24 @@
         <v>-77.409240999999994</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -1493,24 +1493,24 @@
         <v>-77.402915500000006</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -1522,24 +1522,24 @@
         <v>-77.399658203125</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -1551,24 +1551,24 @@
         <v>-77.402915500000006</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -1580,24 +1580,24 @@
         <v>-77.382812299999998</v>
       </c>
       <c r="H26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -1609,24 +1609,24 @@
         <v>-77.384221699999998</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -1638,24 +1638,24 @@
         <v>-77.409240999999994</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -1667,10 +1667,10 @@
         <v>-77.368133999999998</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
my branch w new files ig
</commit_message>
<xml_diff>
--- a/shinyapp/data/Sterling_Youth_Development 3.xlsx
+++ b/shinyapp/data/Sterling_Youth_Development 3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{78C83608-0B1F-D340-BEC4-86EC4F0A89BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A364F354-7501-EB44-8043-F0FE83B1D9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
   </bookViews>
@@ -36,9 +36,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="124">
   <si>
-    <t>Longitude</t>
-  </si>
-  <si>
     <t>Costco</t>
   </si>
   <si>
@@ -183,9 +180,6 @@
     <t>20908 Ashburn Road, Ashburn, VA 20147, United States of America</t>
   </si>
   <si>
-    <t>Latitude</t>
-  </si>
-  <si>
     <t>M-F: 10:00AM - 8:30PM</t>
   </si>
   <si>
@@ -231,9 +225,6 @@
     <t>M-F 7:00AM - 6:00PM</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
     <t>Parks, Recreation and Community Services</t>
   </si>
   <si>
@@ -393,19 +384,28 @@
     <t>Type</t>
   </si>
   <si>
-    <t>Address</t>
-  </si>
-  <si>
-    <t>Website</t>
-  </si>
-  <si>
     <t>Cost</t>
   </si>
   <si>
-    <t>Description</t>
-  </si>
-  <si>
-    <t>Hours</t>
+    <t>Name3</t>
+  </si>
+  <si>
+    <t>Address3</t>
+  </si>
+  <si>
+    <t>Website3</t>
+  </si>
+  <si>
+    <t>Latitude3</t>
+  </si>
+  <si>
+    <t>Longitude3</t>
+  </si>
+  <si>
+    <t>Description3</t>
+  </si>
+  <si>
+    <t>Hours3</t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="I1" sqref="I1"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,25 +840,25 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>65</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
         <v>118</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="E1" t="s">
+        <v>116</v>
+      </c>
+      <c r="F1" t="s">
         <v>120</v>
       </c>
-      <c r="E1" t="s">
+      <c r="G1" t="s">
         <v>121</v>
-      </c>
-      <c r="F1" t="s">
-        <v>49</v>
-      </c>
-      <c r="G1" t="s">
-        <v>0</v>
       </c>
       <c r="H1" t="s">
         <v>122</v>
@@ -869,16 +869,16 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>116</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -890,24 +890,24 @@
         <v>-77.555258699999996</v>
       </c>
       <c r="H2" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>91</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>17</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -919,24 +919,24 @@
         <v>-77.552453999999997</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -948,24 +948,24 @@
         <v>-77.555297999999993</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>94</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -977,24 +977,24 @@
         <v>-77.553653999999995</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I5" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1006,24 +1006,24 @@
         <v>-77.375861999999998</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I6" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1035,24 +1035,24 @@
         <v>-77.358749000000003</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="I7" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1064,24 +1064,24 @@
         <v>-77.3927944</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I8" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1093,21 +1093,21 @@
         <v>-77.486816000000005</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1119,24 +1119,24 @@
         <v>-77.520797999999999</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>90</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1148,24 +1148,24 @@
         <v>-77.310794000000001</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1177,21 +1177,21 @@
         <v>-77.408413999999993</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1203,24 +1203,24 @@
         <v>-77.400994999999995</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I13" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1232,24 +1232,24 @@
         <v>-77.405699999999996</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="I14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1261,24 +1261,24 @@
         <v>-77.565443999999999</v>
       </c>
       <c r="H15" s="5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="I15" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>92</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>14</v>
-      </c>
       <c r="D16" s="2" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -1290,24 +1290,24 @@
         <v>-77.346993999999995</v>
       </c>
       <c r="H16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="I16" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1319,24 +1319,24 @@
         <v>-77.406756999999999</v>
       </c>
       <c r="H17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1348,24 +1348,24 @@
         <v>-77.499871799999994</v>
       </c>
       <c r="H18" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E19" s="2">
         <v>1</v>
@@ -1377,24 +1377,24 @@
         <v>-77.368133999999998</v>
       </c>
       <c r="H19" s="9" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B20" s="2" t="s">
-        <v>89</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>25</v>
-      </c>
       <c r="D20" s="2" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -1406,24 +1406,24 @@
         <v>-77.149856999999997</v>
       </c>
       <c r="H20" s="8" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>83</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
@@ -1435,24 +1435,24 @@
         <v>-77.040006199999993</v>
       </c>
       <c r="H21" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B22" t="s">
+        <v>86</v>
+      </c>
+      <c r="C22" t="s">
+        <v>83</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>70</v>
-      </c>
-      <c r="B22" t="s">
-        <v>89</v>
-      </c>
-      <c r="C22" t="s">
-        <v>86</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>73</v>
       </c>
       <c r="E22" s="2">
         <v>1</v>
@@ -1464,24 +1464,24 @@
         <v>-77.409240999999994</v>
       </c>
       <c r="H22" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="B23" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C23" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D23" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E23" s="2">
         <v>1</v>
@@ -1493,24 +1493,24 @@
         <v>-77.402915500000006</v>
       </c>
       <c r="H23" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="D24" s="12" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
@@ -1522,24 +1522,24 @@
         <v>-77.399658203125</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="B25" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C25" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -1551,24 +1551,24 @@
         <v>-77.402915500000006</v>
       </c>
       <c r="H25" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>85</v>
+        <v>82</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -1580,24 +1580,24 @@
         <v>-77.382812299999998</v>
       </c>
       <c r="H26" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="I26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>84</v>
+        <v>81</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -1609,24 +1609,24 @@
         <v>-77.384221699999998</v>
       </c>
       <c r="H27" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>82</v>
+        <v>79</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -1638,24 +1638,24 @@
         <v>-77.409240999999994</v>
       </c>
       <c r="H28" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>117</v>
+        <v>114</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -1667,10 +1667,10 @@
         <v>-77.368133999999998</v>
       </c>
       <c r="H29" s="7" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="I29" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated code and changes
</commit_message>
<xml_diff>
--- a/shinyapp/data/Sterling_Youth_Development 3.xlsx
+++ b/shinyapp/data/Sterling_Youth_Development 3.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10708"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tayosborne/Downloads/2022_DSPG_Loudoun/shinyapp/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB39AB62-13CE-2F49-948A-0CFD93586747}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A364F354-7501-EB44-8043-F0FE83B1D9B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="15940" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
   </bookViews>
@@ -261,6 +261,9 @@
     <t>YMCA - Rolling Ridge Elementary</t>
   </si>
   <si>
+    <t xml:space="preserve">YMCA  - Guildord Elementary </t>
+  </si>
+  <si>
     <t>Parents want their kids to learn and grow! The Y’s After School Program offers activities and support in homework, sports, fitness, science, art, mathematics, recreation, and reading. We also have fun games that will keep kids engaged and learning!</t>
   </si>
   <si>
@@ -403,9 +406,6 @@
   </si>
   <si>
     <t>Hours3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">YMCA  - Guilford Elementary </t>
   </si>
 </sst>
 </file>
@@ -822,7 +822,7 @@
   <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -840,31 +840,31 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>117</v>
+      </c>
+      <c r="B1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
         <v>116</v>
       </c>
-      <c r="B1" t="s">
-        <v>114</v>
-      </c>
-      <c r="C1" t="s">
-        <v>117</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>118</v>
-      </c>
-      <c r="E1" t="s">
-        <v>115</v>
-      </c>
       <c r="F1" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="G1" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="H1" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="I1" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -872,13 +872,13 @@
         <v>63</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C2" t="s">
         <v>64</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -901,13 +901,13 @@
         <v>15</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -930,13 +930,13 @@
         <v>9</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>46</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -948,7 +948,7 @@
         <v>-77.555297999999993</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
       <c r="I4" t="s">
         <v>54</v>
@@ -959,13 +959,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>41</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>96</v>
+        <v>97</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -988,13 +988,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>42</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1017,13 +1017,13 @@
         <v>5</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>89</v>
+        <v>90</v>
       </c>
       <c r="C7" s="5" t="s">
         <v>43</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1046,13 +1046,13 @@
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>44</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1075,13 +1075,13 @@
         <v>8</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C9" s="4" t="s">
         <v>47</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1101,13 +1101,13 @@
         <v>18</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>19</v>
       </c>
       <c r="D10" s="12" t="s">
-        <v>104</v>
+        <v>105</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1130,13 +1130,13 @@
         <v>28</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="C11" s="2" t="s">
         <v>21</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1159,13 +1159,13 @@
         <v>7</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C12" s="5" t="s">
         <v>45</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1185,13 +1185,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C13" s="5" t="s">
         <v>38</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1214,13 +1214,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C14" s="5" t="s">
         <v>39</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>94</v>
+        <v>95</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1243,13 +1243,13 @@
         <v>2</v>
       </c>
       <c r="B15" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C15" s="5" t="s">
         <v>40</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
       <c r="E15">
         <v>1</v>
@@ -1272,13 +1272,13 @@
         <v>12</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C16" s="2" t="s">
         <v>13</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>92</v>
+        <v>93</v>
       </c>
       <c r="E16" s="2">
         <v>1</v>
@@ -1301,13 +1301,13 @@
         <v>26</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C17" s="2" t="s">
         <v>29</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
@@ -1330,13 +1330,13 @@
         <v>58</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
       <c r="C18" s="2" t="s">
         <v>59</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="E18" s="2">
         <v>0</v>
@@ -1356,16 +1356,16 @@
     </row>
     <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C19" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E19" s="2">
         <v>1</v>
@@ -1380,7 +1380,7 @@
         <v>11</v>
       </c>
       <c r="I19" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
@@ -1388,13 +1388,13 @@
         <v>23</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C20" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="E20" s="2">
         <v>0</v>
@@ -1417,10 +1417,10 @@
         <v>66</v>
       </c>
       <c r="B21" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C21" t="s">
-        <v>79</v>
+        <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>70</v>
@@ -1438,7 +1438,7 @@
         <v>71</v>
       </c>
       <c r="I21" s="2" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
@@ -1446,10 +1446,10 @@
         <v>67</v>
       </c>
       <c r="B22" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C22" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D22" s="12" t="s">
         <v>70</v>
@@ -1467,7 +1467,7 @@
         <v>71</v>
       </c>
       <c r="I22" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
@@ -1475,10 +1475,10 @@
         <v>68</v>
       </c>
       <c r="B23" t="s">
+        <v>86</v>
+      </c>
+      <c r="C23" t="s">
         <v>85</v>
-      </c>
-      <c r="C23" t="s">
-        <v>84</v>
       </c>
       <c r="D23" s="12" t="s">
         <v>70</v>
@@ -1496,7 +1496,7 @@
         <v>71</v>
       </c>
       <c r="I23" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1504,10 +1504,10 @@
         <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C24" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="D24" s="12" t="s">
         <v>70</v>
@@ -1525,7 +1525,7 @@
         <v>71</v>
       </c>
       <c r="I24" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
@@ -1533,13 +1533,13 @@
         <v>72</v>
       </c>
       <c r="B25" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" t="s">
         <v>85</v>
       </c>
-      <c r="C25" t="s">
-        <v>84</v>
-      </c>
       <c r="D25" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
@@ -1551,10 +1551,10 @@
         <v>-77.402915500000006</v>
       </c>
       <c r="H25" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I25" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
@@ -1562,13 +1562,13 @@
         <v>73</v>
       </c>
       <c r="B26" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C26" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="D26" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E26" s="2">
         <v>1</v>
@@ -1580,10 +1580,10 @@
         <v>-77.382812299999998</v>
       </c>
       <c r="H26" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="I26" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
@@ -1591,13 +1591,13 @@
         <v>74</v>
       </c>
       <c r="B27" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C27" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
@@ -1609,24 +1609,24 @@
         <v>-77.384221699999998</v>
       </c>
       <c r="H27" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I27" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>123</v>
+        <v>75</v>
       </c>
       <c r="B28" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C28" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="D28" s="11" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
@@ -1638,24 +1638,24 @@
         <v>-77.409240999999994</v>
       </c>
       <c r="H28" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="I28" t="s">
-        <v>77</v>
+        <v>78</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>106</v>
+        <v>107</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="C29" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="E29" s="2">
         <v>1</v>
@@ -1670,7 +1670,7 @@
         <v>11</v>
       </c>
       <c r="I29" t="s">
-        <v>108</v>
+        <v>109</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
updated youth dev file
</commit_message>
<xml_diff>
--- a/shinyapp/data/Sterling_Youth_Development 3.xlsx
+++ b/shinyapp/data/Sterling_Youth_Development 3.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/amandaljuba/Downloads/DSPG-R-Training/2022_DSPG_Loudoun/shinyapp/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7CCE4397-F25E-BA41-B5A8-5E50D963F4F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{09C6B16B-0B62-EA44-86B8-152841EEEA5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25500" windowHeight="15940" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
+    <workbookView xWindow="5940" yWindow="500" windowWidth="22860" windowHeight="15940" xr2:uid="{0612B967-1994-9F41-A7BC-753ACB378C0D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="120">
   <si>
     <t>Costco</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Apple Federal Credit Union</t>
   </si>
   <si>
-    <t>Irene's Prom Closet</t>
-  </si>
-  <si>
     <t>Loudoun Soccer</t>
   </si>
   <si>
@@ -156,9 +153,6 @@
     <t>21361 Gentry Dr, Sterling, VA 20166</t>
   </si>
   <si>
-    <t>409 Madison Ct SE, Leesburg, VA 20175</t>
-  </si>
-  <si>
     <t>19798 Sycolin Rd, Leesburg, VA 20175</t>
   </si>
   <si>
@@ -219,9 +213,6 @@
     <t>In the Read-Aloud program, volunteers and kids read great books, selected to support a theme such as onomatopoeia, or superheroes or cats and dogs. Kids and adults share conversations and work on an activity related to the books' theme. And every week, the kids pick a new book for their own.</t>
   </si>
   <si>
-    <t>Irene' Prom Closet donates formal attire to high school girls with financial need who otherwise would not be able to attend their schools' dances, homecomings, and proms</t>
-  </si>
-  <si>
     <t>M-F 7:00AM - 6:00PM</t>
   </si>
   <si>
@@ -303,9 +294,6 @@
     <t>Athletics</t>
   </si>
   <si>
-    <t>Resource</t>
-  </si>
-  <si>
     <t>Activity</t>
   </si>
   <si>
@@ -324,9 +312,6 @@
     <t>https://www.applefcu.org/</t>
   </si>
   <si>
-    <t>https://www.irenespromcloset.com/</t>
-  </si>
-  <si>
     <t>https://www.loudounsoccer.com/</t>
   </si>
   <si>
@@ -406,6 +391,9 @@
   </si>
   <si>
     <t>Hours3</t>
+  </si>
+  <si>
+    <t>Other</t>
   </si>
 </sst>
 </file>
@@ -415,7 +403,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -478,6 +466,24 @@
       <charset val="1"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="18"/>
+      <color rgb="FF000000"/>
+      <name val="Helvetica Neue"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -501,7 +507,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="43" fontId="7" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -525,6 +531,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -841,10 +850,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08265865-87B3-A141-B92B-A5F35EC84153}">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="A32" sqref="A32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -862,45 +871,45 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>112</v>
+      </c>
+      <c r="B1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C1" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="E1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F1" t="s">
+        <v>115</v>
+      </c>
+      <c r="G1" t="s">
+        <v>116</v>
+      </c>
+      <c r="H1" t="s">
         <v>117</v>
       </c>
-      <c r="B1" t="s">
-        <v>115</v>
-      </c>
-      <c r="C1" t="s">
+      <c r="I1" t="s">
         <v>118</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>119</v>
-      </c>
-      <c r="E1" t="s">
-        <v>116</v>
-      </c>
-      <c r="F1" t="s">
-        <v>120</v>
-      </c>
-      <c r="G1" t="s">
-        <v>121</v>
-      </c>
-      <c r="H1" t="s">
-        <v>122</v>
-      </c>
-      <c r="I1" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C2" s="13" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
       <c r="E2" s="2">
         <v>1</v>
@@ -912,24 +921,24 @@
         <v>-77.555258699999996</v>
       </c>
       <c r="H2" t="s">
-        <v>65</v>
+        <v>62</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="3" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="B3" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>16</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="E3" s="2">
         <v>1</v>
@@ -941,24 +950,24 @@
         <v>-77.552453999999997</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>44</v>
+      </c>
+      <c r="D4" s="5" t="s">
         <v>88</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>46</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>92</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -970,24 +979,24 @@
         <v>-77.555297999999993</v>
       </c>
       <c r="H4" s="5" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="I4" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C5" s="5" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D5" s="5" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -999,24 +1008,24 @@
         <v>-77.553653999999995</v>
       </c>
       <c r="H5" s="5" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="I5" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="6" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>88</v>
+        <v>85</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D6" s="12" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="E6">
         <v>0</v>
@@ -1028,24 +1037,24 @@
         <v>-77.375861999999998</v>
       </c>
       <c r="H6" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
     </row>
     <row r="7" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>99</v>
+        <v>94</v>
       </c>
       <c r="E7">
         <v>1</v>
@@ -1057,24 +1066,24 @@
         <v>-77.358749000000003</v>
       </c>
       <c r="H7" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I7" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C8" s="5" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1086,24 +1095,24 @@
         <v>-77.3927944</v>
       </c>
       <c r="H8" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="I8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="9" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A9" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" s="10" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C9" s="4" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="E9">
         <v>1</v>
@@ -1115,21 +1124,21 @@
         <v>-77.486816000000005</v>
       </c>
       <c r="H9" s="5" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C10" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C10" s="2" t="s">
-        <v>19</v>
-      </c>
       <c r="D10" s="12" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="E10" s="2">
         <v>1</v>
@@ -1141,24 +1150,24 @@
         <v>-77.520797999999999</v>
       </c>
       <c r="H10" s="7" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="E11" s="2">
         <v>1</v>
@@ -1170,24 +1179,24 @@
         <v>-77.310794000000001</v>
       </c>
       <c r="H11" s="7" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="51" x14ac:dyDescent="0.2">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
       <c r="E12">
         <v>0</v>
@@ -1199,7 +1208,7 @@
         <v>-77.408413999999993</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="13" spans="1:9" ht="34" x14ac:dyDescent="0.2">
@@ -1207,13 +1216,13 @@
         <v>0</v>
       </c>
       <c r="B13" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D13" s="12" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E13">
         <v>1</v>
@@ -1225,10 +1234,10 @@
         <v>-77.400994999999995</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="I13" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
@@ -1236,13 +1245,13 @@
         <v>1</v>
       </c>
       <c r="B14" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D14" s="5" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1254,271 +1263,271 @@
         <v>-77.405699999999996</v>
       </c>
       <c r="H14" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I14" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
-        <v>2</v>
-      </c>
-      <c r="B15" t="s">
+      <c r="A15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="D15" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="D15" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>39.110369400000003</v>
-      </c>
-      <c r="G15">
-        <v>-77.565443999999999</v>
-      </c>
-      <c r="H15" s="5" t="s">
-        <v>61</v>
+      <c r="E15" s="2">
+        <v>1</v>
+      </c>
+      <c r="F15" s="2">
+        <v>38.9531086</v>
+      </c>
+      <c r="G15" s="2">
+        <v>-77.346993999999995</v>
+      </c>
+      <c r="H15" s="8" t="s">
+        <v>13</v>
       </c>
       <c r="I15" t="s">
-        <v>49</v>
+        <v>59</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>13</v>
+        <v>28</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>93</v>
+        <v>106</v>
       </c>
       <c r="E16" s="2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="F16" s="2">
-        <v>38.9531086</v>
+        <v>38.9978257</v>
       </c>
       <c r="G16" s="2">
-        <v>-77.346993999999995</v>
-      </c>
-      <c r="H16" s="8" t="s">
-        <v>14</v>
-      </c>
-      <c r="I16" t="s">
-        <v>62</v>
+        <v>-77.406756999999999</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>55</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
-        <v>26</v>
+        <v>56</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>89</v>
+        <v>119</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>29</v>
+        <v>57</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E17" s="2">
         <v>0</v>
       </c>
-      <c r="F17" s="2">
-        <v>38.9978257</v>
-      </c>
-      <c r="G17" s="2">
-        <v>-77.406756999999999</v>
-      </c>
-      <c r="H17" s="3" t="s">
-        <v>27</v>
+      <c r="F17">
+        <v>38.744839399999996</v>
+      </c>
+      <c r="G17">
+        <v>-77.499871799999994</v>
+      </c>
+      <c r="H17" t="s">
+        <v>58</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="34" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="B18" s="2" t="s">
-        <v>89</v>
+        <v>103</v>
+      </c>
+      <c r="B18" s="5" t="s">
+        <v>83</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>59</v>
+        <v>9</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>112</v>
+        <v>98</v>
       </c>
       <c r="E18" s="2">
+        <v>1</v>
+      </c>
+      <c r="F18" s="2">
+        <v>38.955991699999998</v>
+      </c>
+      <c r="G18" s="2">
+        <v>-77.368133999999998</v>
+      </c>
+      <c r="H18" s="9" t="s">
+        <v>10</v>
+      </c>
+      <c r="I18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>83</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>105</v>
+      </c>
+      <c r="E19" s="2">
         <v>0</v>
       </c>
-      <c r="F18">
-        <v>38.744839399999996</v>
-      </c>
-      <c r="G18">
-        <v>-77.499871799999994</v>
-      </c>
-      <c r="H18" t="s">
-        <v>60</v>
-      </c>
-      <c r="I18" s="2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="34" x14ac:dyDescent="0.2">
-      <c r="A19" s="2" t="s">
-        <v>108</v>
-      </c>
-      <c r="B19" s="5" t="s">
-        <v>86</v>
-      </c>
-      <c r="C19" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D19" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E19" s="2">
-        <v>1</v>
-      </c>
       <c r="F19" s="2">
-        <v>38.955991699999998</v>
+        <v>39.065376299999997</v>
       </c>
       <c r="G19" s="2">
-        <v>-77.368133999999998</v>
-      </c>
-      <c r="H19" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="I19" t="s">
-        <v>109</v>
+        <v>-77.149856999999997</v>
+      </c>
+      <c r="H19" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>54</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>110</v>
+        <v>63</v>
+      </c>
+      <c r="B20" t="s">
+        <v>83</v>
+      </c>
+      <c r="C20" t="s">
+        <v>77</v>
+      </c>
+      <c r="D20" s="12" t="s">
+        <v>67</v>
       </c>
       <c r="E20" s="2">
-        <v>0</v>
-      </c>
-      <c r="F20" s="2">
-        <v>39.065376299999997</v>
-      </c>
-      <c r="G20" s="2">
-        <v>-77.149856999999997</v>
-      </c>
-      <c r="H20" s="8" t="s">
-        <v>25</v>
+        <v>1</v>
+      </c>
+      <c r="F20" s="14">
+        <v>38.996525099999999</v>
+      </c>
+      <c r="G20" s="14">
+        <v>-77.398243500000007</v>
+      </c>
+      <c r="H20" t="s">
+        <v>68</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="B21" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C21" t="s">
         <v>80</v>
       </c>
       <c r="D21" s="12" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="E21" s="2">
         <v>1</v>
       </c>
-      <c r="F21" s="14">
-        <v>38.996525099999999</v>
-      </c>
-      <c r="G21" s="14">
-        <v>-77.398243500000007</v>
+      <c r="F21">
+        <v>38.994826000000003</v>
+      </c>
+      <c r="G21">
+        <v>-77.409240999999994</v>
       </c>
       <c r="H21" t="s">
-        <v>71</v>
-      </c>
-      <c r="I21" s="2" t="s">
-        <v>78</v>
+        <v>68</v>
+      </c>
+      <c r="I21" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B22" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="D22" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="B22" t="s">
-        <v>86</v>
-      </c>
-      <c r="C22" t="s">
-        <v>83</v>
-      </c>
-      <c r="D22" s="12" t="s">
-        <v>70</v>
-      </c>
       <c r="E22" s="2">
         <v>1</v>
       </c>
       <c r="F22">
-        <v>38.994826000000003</v>
+        <v>39.009005999999999</v>
       </c>
       <c r="G22">
-        <v>-77.409240999999994</v>
+        <v>-77.402915500000006</v>
       </c>
       <c r="H22" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="I22" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="B23" t="s">
+        <v>83</v>
+      </c>
+      <c r="C23" t="s">
+        <v>81</v>
+      </c>
+      <c r="D23" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="E23" s="2">
+        <v>1</v>
+      </c>
+      <c r="F23">
+        <v>38.990940093994098</v>
+      </c>
+      <c r="G23">
+        <v>-77.399658203125</v>
+      </c>
+      <c r="H23" t="s">
         <v>68</v>
       </c>
-      <c r="B23" t="s">
-        <v>86</v>
-      </c>
-      <c r="C23" t="s">
-        <v>85</v>
-      </c>
-      <c r="D23" s="12" t="s">
-        <v>70</v>
-      </c>
-      <c r="E23" s="2">
-        <v>1</v>
-      </c>
-      <c r="F23">
-        <v>39.009005999999999</v>
-      </c>
-      <c r="G23">
-        <v>-77.402915500000006</v>
-      </c>
-      <c r="H23" t="s">
-        <v>71</v>
-      </c>
       <c r="I23" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.2">
@@ -1526,184 +1535,185 @@
         <v>69</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C24" t="s">
-        <v>84</v>
-      </c>
-      <c r="D24" s="12" t="s">
-        <v>70</v>
+        <v>82</v>
+      </c>
+      <c r="D24" s="11" t="s">
+        <v>76</v>
       </c>
       <c r="E24" s="2">
         <v>1</v>
       </c>
       <c r="F24">
-        <v>38.990940093994098</v>
+        <v>39.009005999999999</v>
       </c>
       <c r="G24">
-        <v>-77.399658203125</v>
+        <v>-77.402915500000006</v>
       </c>
       <c r="H24" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="I24" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="B25" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C25" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="D25" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E25" s="2">
         <v>1</v>
       </c>
       <c r="F25">
-        <v>39.009005999999999</v>
+        <v>39.036763100000002</v>
       </c>
       <c r="G25">
-        <v>-77.402915500000006</v>
+        <v>-77.382812299999998</v>
       </c>
       <c r="H25" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="I25" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="B26" t="s">
+        <v>83</v>
+      </c>
+      <c r="C26" t="s">
+        <v>78</v>
+      </c>
+      <c r="D26" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="E26" s="2">
+        <v>1</v>
+      </c>
+      <c r="F26">
+        <v>39.015029499999997</v>
+      </c>
+      <c r="G26">
+        <v>-77.384221699999998</v>
+      </c>
+      <c r="H26" t="s">
         <v>73</v>
       </c>
-      <c r="B26" t="s">
-        <v>86</v>
-      </c>
-      <c r="C26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D26" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="E26" s="2">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>39.036763100000002</v>
-      </c>
-      <c r="G26">
-        <v>-77.382812299999998</v>
-      </c>
-      <c r="H26" t="s">
-        <v>77</v>
-      </c>
       <c r="I26" t="s">
-        <v>78</v>
+        <v>75</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B27" t="s">
-        <v>86</v>
+        <v>83</v>
       </c>
       <c r="C27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="D27" s="11" t="s">
-        <v>79</v>
+        <v>76</v>
       </c>
       <c r="E27" s="2">
         <v>1</v>
       </c>
       <c r="F27">
-        <v>39.015029499999997</v>
+        <v>38.994826000000003</v>
       </c>
       <c r="G27">
-        <v>-77.384221699999998</v>
+        <v>-77.409240999999994</v>
       </c>
       <c r="H27" t="s">
-        <v>76</v>
+        <v>73</v>
       </c>
       <c r="I27" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.2">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B28" t="s">
-        <v>86</v>
-      </c>
-      <c r="C28" t="s">
-        <v>83</v>
-      </c>
-      <c r="D28" s="11" t="s">
-        <v>79</v>
+        <v>102</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>98</v>
       </c>
       <c r="E28" s="2">
         <v>1</v>
       </c>
-      <c r="F28">
-        <v>38.994826000000003</v>
-      </c>
-      <c r="G28">
-        <v>-77.409240999999994</v>
-      </c>
-      <c r="H28" t="s">
-        <v>76</v>
+      <c r="F28" s="2">
+        <v>38.955991699999998</v>
+      </c>
+      <c r="G28" s="2">
+        <v>-77.368133999999998</v>
+      </c>
+      <c r="H28" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="I28" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="29" spans="1:9" ht="32" x14ac:dyDescent="0.2">
-      <c r="A29" s="2" t="s">
-        <v>107</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>103</v>
-      </c>
-      <c r="E29" s="2">
-        <v>1</v>
-      </c>
-      <c r="F29" s="2">
-        <v>38.955991699999998</v>
-      </c>
-      <c r="G29" s="2">
-        <v>-77.368133999999998</v>
-      </c>
-      <c r="H29" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="I29" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="D30" s="5"/>
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" ht="23" x14ac:dyDescent="0.25">
+      <c r="A29" s="2"/>
+      <c r="C29" s="15"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="2"/>
+      <c r="H29" s="16"/>
+    </row>
+    <row r="30" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="C30" s="15"/>
+      <c r="E30" s="2"/>
+      <c r="H30" s="17"/>
+    </row>
+    <row r="31" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="C31" s="15"/>
+      <c r="E31" s="2"/>
+    </row>
+    <row r="32" spans="1:9" ht="18" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="C32" s="15"/>
+      <c r="E32" s="2"/>
+    </row>
+    <row r="33" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="C33" s="15"/>
+      <c r="E33" s="2"/>
+    </row>
+    <row r="34" spans="1:5" ht="18" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="C34" s="15"/>
+      <c r="E34" s="2"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="D21" r:id="rId1" display="http://www.loudoun.gov/casa" xr:uid="{DA1323AB-076F-2447-B66A-8156842A9918}"/>
-    <hyperlink ref="D22" r:id="rId2" display="http://www.loudoun.gov/casa" xr:uid="{B2D7ECEF-FAFB-2741-AED0-9969F17C2CD5}"/>
-    <hyperlink ref="D23" r:id="rId3" display="http://www.loudoun.gov/casa" xr:uid="{772C6E6C-0B95-E74A-9330-EFE23FC4ACD5}"/>
-    <hyperlink ref="D24" r:id="rId4" display="http://www.loudoun.gov/casa" xr:uid="{90676448-C463-D542-AAEF-1ACC8D8AB413}"/>
+    <hyperlink ref="D20" r:id="rId1" display="http://www.loudoun.gov/casa" xr:uid="{DA1323AB-076F-2447-B66A-8156842A9918}"/>
+    <hyperlink ref="D21" r:id="rId2" display="http://www.loudoun.gov/casa" xr:uid="{B2D7ECEF-FAFB-2741-AED0-9969F17C2CD5}"/>
+    <hyperlink ref="D22" r:id="rId3" display="http://www.loudoun.gov/casa" xr:uid="{772C6E6C-0B95-E74A-9330-EFE23FC4ACD5}"/>
+    <hyperlink ref="D23" r:id="rId4" display="http://www.loudoun.gov/casa" xr:uid="{90676448-C463-D542-AAEF-1ACC8D8AB413}"/>
     <hyperlink ref="D13" r:id="rId5" xr:uid="{9C3C10A0-326B-EC44-946E-7252A8A359B5}"/>
     <hyperlink ref="D6" r:id="rId6" xr:uid="{A18F176E-9BC6-C645-B7C6-0CB48574C44C}"/>
     <hyperlink ref="D10" r:id="rId7" xr:uid="{E66D4200-6061-7E44-9B93-87E46D184339}"/>

</xml_diff>